<commit_message>
fix, test: fix bus routing error & add regression test directory
- only a few changes in mazererouter.cc
- a new function path_length for length calculation strategy
- new functions in config/trans_xlsx_to_json.py, for transforming excel
  into JSONs with a new way to calculate track coordinates
- divide test to simpletest and regressiontest
</commit_message>
<xml_diff>
--- a/test/regression_test/case2/case2.xlsx
+++ b/test/regression_test/case2/case2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FDUFiles\Tao_group\kiwi\jsy_version_kiwi\修改2024-08-26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FDUFiles\Tao_group\kiwi\MyKiwi\test\regression_test\case2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726DF7CF-2B3D-4913-91DD-E49BCBB59EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70FCB3-CEDE-4D3A-B02C-8C83ED4F51E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3215,8 +3215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68954699-C253-4E24-923F-26F80023EC59}">
   <dimension ref="A1:C679"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3375,17 +3375,7 @@
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="C15" s="16">
-        <v>-1</v>
-      </c>
-    </row>
+    <row r="15" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>374</v>
@@ -3985,9 +3975,15 @@
       <c r="C73" s="16"/>
     </row>
     <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="16"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
+      <c r="A74" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="C74" s="16">
+        <v>-1</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16"/>

</xml_diff>